<commit_message>
add bfm manual citation
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145D5796-33DA-9749-B2EE-A593F02377E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FACD729-0F65-004D-AE57-13F2ADBB9C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -223,6 +223,31 @@
   </si>
   <si>
     <t>madec_2017</t>
+  </si>
+  <si>
+    <t>bfm_2020</t>
+  </si>
+  <si>
+    <t>"@misc{
+  author       = {Vichi Marcello and
+                  Tomas Lovato and
+                  Momme Butenschön and
+                  Letizia Tedesco and
+                  Paolo Lazzari and
+                  Gianpiero Cossarini and
+                  Simona Masina and
+                  Nadia Pinardi and
+                  Cosimo Solidoro and
+                  Marco Zavatarelli},
+  title        = {he Biogeochemical Flux Model (BFM): Equation Description and User Manual. BFM version 5.2},
+  month        = jun,
+  year         = 2017,
+  version      = {v5.2},
+  url          = {https://cmcc-foundation.github.io/www.bfm-community.eu/files/bfm-V5.2.0-manual_r1.2_202006.pdf}
+}"</t>
+  </si>
+  <si>
+    <t>www.bfm-community.eu</t>
   </si>
 </sst>
 </file>
@@ -2487,8 +2512,8 @@
   </sheetPr>
   <dimension ref="A1:IP52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2620,10 +2645,16 @@
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
add citations and info for cmip6_cmcc_cmcc-cm2-sr5_atmos
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FACD729-0F65-004D-AE57-13F2ADBB9C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AF73CB-D8B7-404F-95CF-40CC3C045C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
     <sheet name="Example" sheetId="2" r:id="rId2"/>
     <sheet name="Citations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -248,6 +248,197 @@
   </si>
   <si>
     <t>www.bfm-community.eu</t>
+  </si>
+  <si>
+    <t>batjes2006soil</t>
+  </si>
+  <si>
+    <t>@article{
+  title={Soil carbon stocks of Jordan and projected changes upon improved management of croplands},
+  author={Batjes, Niels H},
+  journal={Geoderma},
+  volume={132},
+  number={3-4},
+  pages={361--371},
+  year={2006},
+  publisher={Elsevier}
+}'</t>
+  </si>
+  <si>
+    <t>hugelius2012spatial</t>
+  </si>
+  <si>
+    <t>10.1016/j.geoderma.2005.05.013</t>
+  </si>
+  <si>
+    <t>@article{
+  title={Spatial upscaling using thematic maps: An analysis of uncertainties in permafrost soil carbon estimates},
+  author={Hugelius, Gustaf},
+  journal={Global Biogeochemical Cycles},
+  volume={26},
+  number={2},
+  year={2012},
+  publisher={Wiley Online Library}
+}'</t>
+  </si>
+  <si>
+    <t>10.1029/2011GB004154</t>
+  </si>
+  <si>
+    <t>Neale_2012</t>
+  </si>
+  <si>
+    <t>https://www.cesm.ucar.edu/models/cesm1.0/cam/docs/description/cam5_desc.pdf</t>
+  </si>
+  <si>
+    <t>"@article{
+author = {Neale, R. B.  and Gettelman, A. and Park, S. and others},
+title = {Description of the NCAR Community Atmosphere Model (CAM 5.0)},
+journal = {NCAR Technical Note},
+volume = {},
+number = {},
+pages = {},
+Doi = {},
+year = {2012}
+}"</t>
+  </si>
+  <si>
+    <t>Charlton-Perez_2013</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/jgrd.50125</t>
+  </si>
+  <si>
+    <t>Craig_2012</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/1094342011428141</t>
+  </si>
+  <si>
+    <t>Richter_2014</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/2013MS000303</t>
+  </si>
+  <si>
+    <t>Lin-Rood_1996</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/1520-0493(1996)124%3C2046:MFFSLT%3E2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Lin-Rood_1997</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/qj.49712354416</t>
+  </si>
+  <si>
+    <t>Iacono_2008</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/2008JD009944</t>
+  </si>
+  <si>
+    <t>Mlawer_1997</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/97JD00237</t>
+  </si>
+  <si>
+    <t>Pincus-Morcrette_2003</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/2002JD003322</t>
+  </si>
+  <si>
+    <t>Bretherton-Park_2009</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2008JCLI2556.1</t>
+  </si>
+  <si>
+    <t>Zhang-McFarlane_1995</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/07055900.1995.9649539</t>
+  </si>
+  <si>
+    <t>Richter-Rasch_2008</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2007JCLI1789.1</t>
+  </si>
+  <si>
+    <t>Raymond-Blyth_1986</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/1520-0469(1986)043%3C2708:ASMMFN%3E2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Raymond-Blyth_1992</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/1520-0469(1992)049%3C1968:EOTSMM%3E2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Park-Bretherton_2009</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2008JCLI2557.1</t>
+  </si>
+  <si>
+    <t>Morrison-Gettelman_2008</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2008JCLI2105.1</t>
+  </si>
+  <si>
+    <t>Gettelman_2008</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2008JCLI2116.1</t>
+  </si>
+  <si>
+    <t>Gettelman_2010</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/2009JD013797</t>
+  </si>
+  <si>
+    <t>Park_2014</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/JCLI-D-14-00087.1</t>
+  </si>
+  <si>
+    <t>McFarlane_1987</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/1520-0469(1987)044%3C1775:TEOOEG%3E2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Lindzen_1981</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/JC086iC10p09707</t>
+  </si>
+  <si>
+    <t>Richter_2010</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1175/2009JAS3112.1</t>
+  </si>
+  <si>
+    <t>Hoskins_1982</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1146/annurev.fl.14.010182.001023</t>
+  </si>
+  <si>
+    <t>Beres_2005</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/2004JD005504</t>
   </si>
 </sst>
 </file>
@@ -333,6 +524,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -476,7 +668,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -575,6 +767,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2510,10 +2705,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP52"/>
+  <dimension ref="A1:IP50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2658,186 +2853,296 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="15"/>
+      <c r="A10" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
     <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
+      <c r="A15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>58</v>
+      </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
+      <c r="A16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>60</v>
+      </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>64</v>
+      </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="A20" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
+      <c r="A21" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="17"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="17"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="17"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="17"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="A28" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="17"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="17"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="17"/>
-      <c r="B31" s="22"/>
+      <c r="A31" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>90</v>
+      </c>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="17"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>92</v>
+      </c>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="17"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>94</v>
+      </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="17"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
+      <c r="A34" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="17"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
+      <c r="A35" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17"/>
@@ -2943,20 +3248,6 @@
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
-    </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="17"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-    </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="17"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add info for cmip6_cmcc_cmcc-cm2-sr5_aerosol
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F8393C-806D-0E4E-A84B-827B1139F7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280C1BE2-1577-6D44-BEF1-3C2EFCEA3CEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="163">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -738,6 +738,42 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/abs/pii/S0022169404001404</t>
+  </si>
+  <si>
+    <t>Liu_2012</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/gmd-5-709-2012</t>
+  </si>
+  <si>
+    <t>Lamarque_2010</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/acp-10-7017-2010</t>
+  </si>
+  <si>
+    <t>Bond_2007</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1029/2006GB002840</t>
+  </si>
+  <si>
+    <t>Junker-Liousse_2008</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/acp-8-1195-2008</t>
+  </si>
+  <si>
+    <t>Smith_2001</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0921-8181(00)00057-6</t>
+  </si>
+  <si>
+    <t>Smith_2004</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2172/15020102</t>
   </si>
 </sst>
 </file>
@@ -3004,10 +3040,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP52"/>
+  <dimension ref="A1:IP59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3443,230 +3479,307 @@
       <c r="D35" s="23"/>
       <c r="E35" s="23"/>
     </row>
-    <row r="36" spans="1:5" ht="154" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>98</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>101</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>105</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>108</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>112</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E41" s="22"/>
+      <c r="A41" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E42" s="22"/>
-    </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" ht="154" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D44" s="22"/>
+        <v>100</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>101</v>
+      </c>
       <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="C45" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D45" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>105</v>
+      </c>
       <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>130</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B46" s="22"/>
       <c r="C46" s="22" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="E46" s="22"/>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B47" s="22"/>
+        <v>109</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="C47" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D47" s="22"/>
+        <v>111</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>112</v>
+      </c>
       <c r="E47" s="22"/>
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="22"/>
+        <v>113</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>114</v>
+      </c>
       <c r="C48" s="22" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" s="22"/>
+        <v>117</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="C49" s="22" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="22"/>
+    </row>
+    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+    </row>
+    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+    </row>
+    <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="22"/>
+    </row>
+    <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+    </row>
+    <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="22"/>
+    </row>
+    <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" s="22"/>
+    </row>
+    <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B57" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C57" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D57" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="22"/>
-    </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="18" t="s">
+      <c r="E57" s="22"/>
+    </row>
+    <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C58" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="18" t="s">
+    <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B59" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C59" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D59" s="18" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add first version of cmcc-cm2-sr5 seaice (partial) and coupling
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280C1BE2-1577-6D44-BEF1-3C2EFCEA3CEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A192B4-30B1-B843-B13F-C60336DC8BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Example" sheetId="2" r:id="rId2"/>
     <sheet name="Citations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="174">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -774,6 +774,52 @@
   </si>
   <si>
     <t>https://doi.org/10.2172/15020102</t>
+  </si>
+  <si>
+    <t>hunke_2010</t>
+  </si>
+  <si>
+    <t>@article{
+  title={CICE: the Los Alamos Sea Ice Model Documentation and Software User’s Manual Version 4.1 LA-CC-06-012},
+  author={Hunke, Elizabeth C and Lipscomb, William H and Turner, Adrian K and Jeffery, Nicole and Elliott, Scott},
+  journal={T-3 Fluid Dynamics Group, Los Alamos National Laboratory},
+  volume={675},
+  pages={500},
+  year={2010}
+}'</t>
+  </si>
+  <si>
+    <t>https://csdms.colorado.edu/w/images/CICE_documentation_and_software_user's_manual.pdf</t>
+  </si>
+  <si>
+    <t>10.5065/D6B27S71</t>
+  </si>
+  <si>
+    <t>briegleb_2007</t>
+  </si>
+  <si>
+    <t>hunke_1997</t>
+  </si>
+  <si>
+    <t>10.1175/1520-0485(1997)027&lt;1849:AEVPMF&gt;2.0.CO;2</t>
+  </si>
+  <si>
+    <t>lipscomb_2004</t>
+  </si>
+  <si>
+    <t>10.1175/1520-0493(2004)132&lt;1341:MSITUI&gt;2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Assur_1958</t>
+  </si>
+  <si>
+    <t>@book{
+  title={Composition of sea ice and its tensile strength},
+  author={Assur, Andrew},
+  volume={44},
+  year={1960},
+  publisher={US Army Snow, Ice and Permafrost Research Establishment}
+}'</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1049,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1106,6 +1152,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3040,10 +3089,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP59"/>
+  <dimension ref="A1:IP64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3189,89 +3238,90 @@
     </row>
     <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="B10" s="16"/>
-      <c r="C10" s="16" t="s">
-        <v>48</v>
+      <c r="C10" s="34" t="s">
+        <v>164</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+        <v>168</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
+        <v>170</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+        <v>167</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
+        <v>172</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -3279,10 +3329,10 @@
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -3290,76 +3340,76 @@
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="A20" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="A21" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="A22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="A24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -3367,10 +3417,10 @@
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -3378,10 +3428,10 @@
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -3389,102 +3439,98 @@
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+        <v>73</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+        <v>77</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+        <v>79</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
+        <v>81</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="A34" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
+      <c r="A35" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>152</v>
+        <v>90</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -3492,10 +3538,10 @@
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
@@ -3503,283 +3549,342 @@
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
+      <c r="A39" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
+      <c r="A40" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C41" s="34"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="A41" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="C42" s="34"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-    </row>
-    <row r="43" spans="1:5" ht="154" x14ac:dyDescent="0.15">
+      <c r="A42" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>98</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>101</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>105</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="22"/>
+      <c r="A46" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="22"/>
-    </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" ht="154" x14ac:dyDescent="0.15">
       <c r="A48" s="17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>118</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B49" s="22"/>
       <c r="C49" s="22" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="E50" s="22"/>
     </row>
     <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D51" s="22"/>
+        <v>107</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>108</v>
+      </c>
       <c r="E51" s="22"/>
     </row>
     <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B52" s="22"/>
+        <v>109</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="C52" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" s="22"/>
+        <v>111</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>112</v>
+      </c>
       <c r="E52" s="22"/>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B54" s="22"/>
+        <v>117</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="C54" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="22"/>
+        <v>119</v>
+      </c>
+      <c r="D54" s="22" t="s">
+        <v>120</v>
+      </c>
       <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="C55" s="22" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="E55" s="22"/>
     </row>
     <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="17" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B56" s="22"/>
       <c r="C56" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>140</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D56" s="22"/>
       <c r="E56" s="22"/>
     </row>
     <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+    </row>
+    <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="22"/>
+    </row>
+    <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+    </row>
+    <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="E60" s="22"/>
+    </row>
+    <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E61" s="22"/>
+    </row>
+    <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B62" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C57" s="22" t="s">
+      <c r="C62" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D62" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E57" s="22"/>
-    </row>
-    <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="18" t="s">
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C63" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="18" t="s">
+    <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B64" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C64" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D64" s="18" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add few details to cmip6_cmcc_cmcc-cm2-sr5_seaice
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A192B4-30B1-B843-B13F-C60336DC8BE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E431DF0-2C17-0C48-B23E-E133144750DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -810,9 +810,6 @@
     <t>10.1175/1520-0493(2004)132&lt;1341:MSITUI&gt;2.0.CO;2</t>
   </si>
   <si>
-    <t>Assur_1958</t>
-  </si>
-  <si>
     <t>@book{
   title={Composition of sea ice and its tensile strength},
   author={Assur, Andrew},
@@ -820,6 +817,9 @@
   year={1960},
   publisher={US Army Snow, Ice and Permafrost Research Establishment}
 }'</t>
+  </si>
+  <si>
+    <t>assur_1958</t>
   </si>
 </sst>
 </file>
@@ -3092,7 +3092,7 @@
   <dimension ref="A1:IP64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3284,11 +3284,11 @@
     </row>
     <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>

</xml_diff>

<commit_message>
update ocean description for HR4 and VHR4 configurations
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cmcc_citations.xlsx
+++ b/cmip6/citations/cmip6_cmcc_citations.xlsx
@@ -1,36 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/citations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/es-doc.cmcc/cmip6/citations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E431DF0-2C17-0C48-B23E-E133144750DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438C6771-C9CA-9348-BE4F-5DAD4B3B1D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38280" windowHeight="21920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
     <sheet name="Example" sheetId="2" r:id="rId2"/>
     <sheet name="Citations" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="178">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -821,12 +813,33 @@
   <si>
     <t>assur_1958</t>
   </si>
+  <si>
+    <t>scoccimarro_2021</t>
+  </si>
+  <si>
+    <t>10.5194/gmd-2021-294</t>
+  </si>
+  <si>
+    <t>https://gmd.copernicus.org/preprints/gmd-2021-294/</t>
+  </si>
+  <si>
+    <t>"Article{gmd-2021-294,
+AUTHOR = {Scoccimarro, E. and Peano, D. and Gualdi, S. and Bellucci, A. and Lovato, T. and Fogli, P. G. and Navarra, A.},
+TITLE = {Extreme Events Representation in CMCC-CM2 High and Very-High Resolution General Circulation Models},
+JOURNAL = {Geoscientific Model Development Discussions},
+VOLUME = {2021},
+YEAR = {2021},
+PAGES = {1--18},
+URL = {https://gmd.copernicus.org/preprints/gmd-2021-294/},
+DOI = {10.5194/gmd-2021-294}
+}"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -904,6 +917,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF464646"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -1049,7 +1068,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1154,6 +1173,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3089,10 +3111,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP64"/>
+  <dimension ref="A1:IP65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3167,105 +3189,109 @@
       </c>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:250" ht="140" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:250" ht="168" x14ac:dyDescent="0.15">
       <c r="A5" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:250" ht="140" x14ac:dyDescent="0.15">
+      <c r="A6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:250" ht="154" x14ac:dyDescent="0.15">
-      <c r="A6" s="15" t="s">
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:250" ht="154" x14ac:dyDescent="0.15">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B7" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D7" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B8" s="16"/>
       <c r="C8" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>35</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>35</v>
       </c>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>165</v>
+        <v>37</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+        <v>163</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="23"/>
@@ -3273,10 +3299,10 @@
     </row>
     <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>166</v>
+        <v>170</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>171</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="23"/>
@@ -3284,55 +3310,55 @@
     </row>
     <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="34" t="s">
-        <v>172</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="34"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="B15" s="23"/>
-      <c r="C15" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>47</v>
-      </c>
+      <c r="C15" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+        <v>46</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -3340,10 +3366,10 @@
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -3351,10 +3377,10 @@
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -3362,10 +3388,10 @@
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -3373,10 +3399,10 @@
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -3384,10 +3410,10 @@
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -3395,32 +3421,32 @@
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
     </row>
     <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="A25" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -3428,10 +3454,10 @@
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -3439,10 +3465,10 @@
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
@@ -3450,10 +3476,10 @@
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -3461,10 +3487,10 @@
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -3472,10 +3498,10 @@
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
@@ -3483,10 +3509,10 @@
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -3494,21 +3520,21 @@
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
+        <v>81</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
@@ -3516,10 +3542,10 @@
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -3527,10 +3553,10 @@
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
@@ -3538,10 +3564,10 @@
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
@@ -3549,58 +3575,58 @@
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
+      <c r="A39" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>43</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
+      <c r="A41" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
@@ -3608,10 +3634,10 @@
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="17" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>154</v>
+        <v>54</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
@@ -3619,10 +3645,10 @@
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
@@ -3630,268 +3656,279 @@
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="34"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
+      <c r="A46" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>162</v>
+        <v>159</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>160</v>
       </c>
       <c r="C47" s="34"/>
       <c r="D47" s="23"/>
       <c r="E47" s="23"/>
     </row>
-    <row r="48" spans="1:5" ht="154" x14ac:dyDescent="0.15">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C48" s="34"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:5" ht="154" x14ac:dyDescent="0.15">
+      <c r="A49" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B49" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C49" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D49" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="E48" s="22"/>
-    </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>101</v>
       </c>
       <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>103</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B50" s="22"/>
       <c r="C50" s="22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E50" s="22"/>
     </row>
     <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>103</v>
+      </c>
       <c r="C51" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E51" s="22"/>
     </row>
     <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B52" s="22" t="s">
-        <v>110</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B52" s="22"/>
       <c r="C52" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E52" s="22"/>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E55" s="22"/>
     </row>
     <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="C56" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D56" s="22"/>
+        <v>123</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>124</v>
+      </c>
       <c r="E56" s="22"/>
     </row>
     <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B57" s="22"/>
       <c r="C57" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
     </row>
     <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>130</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B58" s="22"/>
       <c r="C58" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>132</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D58" s="22"/>
       <c r="E58" s="22"/>
     </row>
     <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="B59" s="22"/>
+        <v>129</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>130</v>
+      </c>
       <c r="C59" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D59" s="22"/>
+        <v>131</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>132</v>
+      </c>
       <c r="E59" s="22"/>
     </row>
     <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>137</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="D60" s="22"/>
       <c r="E60" s="22"/>
     </row>
     <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="17" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B61" s="22"/>
       <c r="C61" s="22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E61" s="22"/>
     </row>
     <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="E62" s="22"/>
+    </row>
+    <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B63" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C63" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D63" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E62" s="22"/>
-    </row>
-    <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>146</v>
-      </c>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B65" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D65" s="18" t="s">
         <v>150</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{AC67B226-01D9-0347-8104-A630E27AFB74}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{836639C3-72D1-A84B-A294-7235D530CA87}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{AC67B226-01D9-0347-8104-A630E27AFB74}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{836639C3-72D1-A84B-A294-7235D530CA87}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
   <pageSetup orientation="portrait"/>

</xml_diff>